<commit_message>
worked on Time series.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ModelingTools\ModelMuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753E2CD0-2FBB-4DE0-A9B8-21969C7D3398}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37D6CA9-98B4-4F69-80CD-FAAA62100F4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="564" yWindow="348" windowWidth="16884" windowHeight="11652" xr2:uid="{FCA78F46-E8A2-4A0B-99C5-ED3D180C0771}"/>
+    <workbookView minimized="1" xWindow="564" yWindow="348" windowWidth="16884" windowHeight="11652" xr2:uid="{FCA78F46-E8A2-4A0B-99C5-ED3D180C0771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Package or feature</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Total (days) (5 hours per day)</t>
+  </si>
+  <si>
+    <t>Actual (days)</t>
   </si>
 </sst>
 </file>
@@ -540,11 +543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3951DA-3CB1-4991-A5D9-1B38B3B6C84D}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +559,7 @@
     <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +584,11 @@
       <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -596,7 +602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -606,8 +612,11 @@
       <c r="H3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -620,8 +629,11 @@
       <c r="H4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -638,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -652,7 +664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -669,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -683,7 +695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -700,7 +712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -714,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -731,7 +743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -748,7 +760,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -771,7 +783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -794,7 +806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -817,7 +829,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -840,7 +852,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -863,7 +875,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -886,7 +898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -900,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -914,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -927,8 +939,11 @@
       <c r="H21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -942,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -956,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -973,7 +988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1013,7 +1028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1033,7 +1048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1053,7 +1068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1073,7 +1088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1113,7 +1128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
worked on exporting time series files.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ModelingTools\ModelMuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37D6CA9-98B4-4F69-80CD-FAAA62100F4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143CCE37-E087-4917-B1D5-6427CC84B1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="564" yWindow="348" windowWidth="16884" windowHeight="11652" xr2:uid="{FCA78F46-E8A2-4A0B-99C5-ED3D180C0771}"/>
+    <workbookView xWindow="576" yWindow="348" windowWidth="21384" windowHeight="11652" xr2:uid="{FCA78F46-E8A2-4A0B-99C5-ED3D180C0771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
     <t>Total (days) (5 hours per day)</t>
   </si>
   <si>
-    <t>Actual (days)</t>
+    <t>Actual (hours)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>2.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -630,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="I4">
-        <v>1.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -940,7 +940,7 @@
         <v>4</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1106,6 +1106,9 @@
       </c>
       <c r="H30">
         <v>8</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on importing time series files.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ModelingTools\ModelMuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143CCE37-E087-4917-B1D5-6427CC84B1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AF8D7D-E0D7-460C-8027-0D61E263FC5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="576" yWindow="348" windowWidth="21384" windowHeight="11652" xr2:uid="{FCA78F46-E8A2-4A0B-99C5-ED3D180C0771}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on importing time series data.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ModelingTools\ModelMuse\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AF8D7D-E0D7-460C-8027-0D61E263FC5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="348" windowWidth="21384" windowHeight="11652" xr2:uid="{FCA78F46-E8A2-4A0B-99C5-ED3D180C0771}"/>
+    <workbookView xWindow="570" yWindow="345" windowWidth="21390" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -186,7 +180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,31 +529,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3951DA-3CB1-4991-A5D9-1B38B3B6C84D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,7 +582,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -602,7 +596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -613,10 +607,10 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -633,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -650,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -664,7 +658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -681,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -695,7 +689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -712,7 +706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -726,7 +720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -743,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -760,7 +754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -783,7 +777,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -806,7 +800,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -829,7 +823,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -852,7 +846,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -875,7 +869,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -898,7 +892,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -912,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -926,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -943,7 +937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -957,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -971,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -988,7 +982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1008,7 +1002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1028,7 +1022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1048,7 +1042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1068,7 +1062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1088,7 +1082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1131,7 +1125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1148,7 +1142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1168,7 +1162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1188,7 +1182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1205,7 +1199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1217,7 +1211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1225,7 +1219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1234,7 +1228,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1243,7 +1237,7 @@
         <v>166.4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1252,7 +1246,7 @@
         <v>232.95999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Worked on implementing time series in CHD, DRN, GHB, RCH, RIV, and WEL packages.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,7 +541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1001,6 +1001,9 @@
       <c r="H25">
         <v>8</v>
       </c>
+      <c r="I25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1021,6 +1024,9 @@
       <c r="H26">
         <v>8</v>
       </c>
+      <c r="I26">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1105,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1123,6 +1129,9 @@
       </c>
       <c r="H31">
         <v>8</v>
+      </c>
+      <c r="I31">
+        <v>0.75</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1141,8 +1150,11 @@
       <c r="H32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1161,8 +1173,11 @@
       <c r="H33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1182,7 +1197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1199,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1219,7 +1234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1228,7 +1243,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1237,7 +1252,7 @@
         <v>166.4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1246,7 +1261,7 @@
         <v>232.95999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Worked on Time Series for RCH and EVT in MODFLOW 6.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,7 +541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1174,7 +1174,7 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1196,6 +1196,9 @@
       <c r="H34">
         <v>8</v>
       </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -1232,6 +1235,9 @@
       </c>
       <c r="H37">
         <v>16</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on times sseries of MAW, CSUB, SFR, LAK, and UZF packages. Worked on supporting times series in the formula editor.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,7 +541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -981,6 +981,9 @@
       <c r="H24">
         <v>8</v>
       </c>
+      <c r="I24">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1047,6 +1050,9 @@
       <c r="H27">
         <v>16</v>
       </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1067,6 +1073,9 @@
       <c r="H28">
         <v>16</v>
       </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1087,6 +1096,9 @@
       <c r="H29">
         <v>16</v>
       </c>
+      <c r="I29">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1216,6 +1228,9 @@
       <c r="H35">
         <v>8</v>
       </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -1248,6 +1263,10 @@
         <f>SUM(H2:H37)</f>
         <v>832</v>
       </c>
+      <c r="I39">
+        <f t="shared" ref="I39:J39" si="0">SUM(I2:I37)</f>
+        <v>82.5</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1257,6 +1276,10 @@
         <f>H39/5</f>
         <v>166.4</v>
       </c>
+      <c r="I40">
+        <f t="shared" ref="I40:J40" si="1">I39/5</f>
+        <v>16.5</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1266,6 +1289,10 @@
         <f>H40*7/5</f>
         <v>232.95999999999998</v>
       </c>
+      <c r="I41">
+        <f t="shared" ref="I41:J41" si="2">I40*7/5</f>
+        <v>23.1</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1274,6 +1301,10 @@
       <c r="H42">
         <f>H41/30</f>
         <v>7.7653333333333325</v>
+      </c>
+      <c r="I42">
+        <f t="shared" ref="I42:J42" si="3">I41/30</f>
+        <v>0.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on allowing MF6 Time Series in Edit Feature Formula dialog box.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1264,8 +1264,8 @@
         <v>832</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:J39" si="0">SUM(I2:I37)</f>
-        <v>82.5</v>
+        <f t="shared" ref="I39" si="0">SUM(I2:I37)</f>
+        <v>87.5</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,8 +1277,8 @@
         <v>166.4</v>
       </c>
       <c r="I40">
-        <f t="shared" ref="I40:J40" si="1">I39/5</f>
-        <v>16.5</v>
+        <f t="shared" ref="I40" si="1">I39/5</f>
+        <v>17.5</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1290,8 +1290,8 @@
         <v>232.95999999999998</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I41:J41" si="2">I40*7/5</f>
-        <v>23.1</v>
+        <f t="shared" ref="I41" si="2">I40*7/5</f>
+        <v>24.5</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,8 +1303,8 @@
         <v>7.7653333333333325</v>
       </c>
       <c r="I42">
-        <f t="shared" ref="I42:J42" si="3">I41/30</f>
-        <v>0.77</v>
+        <f t="shared" ref="I42" si="3">I41/30</f>
+        <v>0.81666666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on MODFLOW 6 Time Series.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,7 +541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="I39">
         <f t="shared" ref="I39" si="0">SUM(I2:I37)</f>
-        <v>87.5</v>
+        <v>91.5</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="I40">
         <f t="shared" ref="I40" si="1">I39/5</f>
-        <v>17.5</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="I41">
         <f t="shared" ref="I41" si="2">I40*7/5</f>
-        <v>24.5</v>
+        <v>25.619999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="I42">
         <f t="shared" ref="I42" si="3">I41/30</f>
-        <v>0.81666666666666665</v>
+        <v>0.85399999999999987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on MF6 Times series. Planned MF6 solute transport.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Package or feature</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Actual (hours)</t>
+  </si>
+  <si>
+    <t>TS estimate</t>
+  </si>
+  <si>
+    <t>TS Actual</t>
   </si>
 </sst>
 </file>
@@ -218,11 +224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +560,7 @@
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +588,14 @@
       <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -596,7 +609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -609,8 +622,14 @@
       <c r="I3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -626,8 +645,14 @@
       <c r="I4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -644,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -658,7 +683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -675,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -689,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -706,7 +731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -720,7 +745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -737,7 +762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -754,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -777,7 +802,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -800,7 +825,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -823,7 +848,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -846,7 +871,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -869,7 +894,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -892,7 +917,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -906,7 +931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -920,7 +945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -936,8 +961,14 @@
       <c r="I21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -951,7 +982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -965,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -984,8 +1015,14 @@
       <c r="I24">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1007,8 +1044,14 @@
       <c r="I25">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>8</v>
+      </c>
+      <c r="K25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1030,8 +1073,14 @@
       <c r="I26">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <v>8</v>
+      </c>
+      <c r="K26">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1053,8 +1102,14 @@
       <c r="I27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>16</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1076,8 +1131,14 @@
       <c r="I28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <v>16</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1099,8 +1160,14 @@
       <c r="I29">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <v>16</v>
+      </c>
+      <c r="K29">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1122,8 +1189,14 @@
       <c r="I30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>8</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1145,8 +1218,14 @@
       <c r="I31">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>8</v>
+      </c>
+      <c r="K31">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1165,8 +1244,14 @@
       <c r="I32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>8</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1188,8 +1273,14 @@
       <c r="I33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>8</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1211,8 +1302,14 @@
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>8</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1231,8 +1328,14 @@
       <c r="I35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>8</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1244,7 +1347,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1254,8 +1357,14 @@
       <c r="I37">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>16</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1264,11 +1373,19 @@
         <v>832</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39" si="0">SUM(I2:I37)</f>
+        <f t="shared" ref="I39:K39" si="0">SUM(I2:I37)</f>
         <v>91.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1281,7 +1398,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1294,7 +1411,7 @@
         <v>25.619999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1305,6 +1422,12 @@
       <c r="I42">
         <f t="shared" ref="I42" si="3">I41/30</f>
         <v>0.85399999999999987</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J43" s="2">
+        <f>K39/J39</f>
+        <v>0.58653846153846156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed undo for time series.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -536,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,8 +547,8 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J3">
         <v>4</v>
       </c>
       <c r="K3">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="I39">
         <f t="shared" ref="I39:K39" si="0">SUM(I2:I37)</f>
-        <v>91.5</v>
+        <v>95.5</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="I40">
         <f t="shared" ref="I40" si="1">I39/5</f>
-        <v>18.3</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="I41">
         <f t="shared" ref="I41" si="2">I40*7/5</f>
-        <v>25.619999999999997</v>
+        <v>26.740000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1421,13 +1421,13 @@
       </c>
       <c r="I42">
         <f t="shared" ref="I42" si="3">I41/30</f>
-        <v>0.85399999999999987</v>
+        <v>0.89133333333333342</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J43" s="2">
         <f>K39/J39</f>
-        <v>0.58653846153846156</v>
+        <v>0.61217948717948723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on package names for solute transport in MF6.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -536,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,8 +547,8 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J3">
         <v>4</v>
       </c>
       <c r="K3">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="I39">
         <f t="shared" ref="I39:K39" si="0">SUM(I2:I37)</f>
-        <v>95.5</v>
+        <v>101.5</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
-        <v>95.5</v>
+        <v>101.5</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="I40">
         <f t="shared" ref="I40" si="1">I39/5</f>
-        <v>19.100000000000001</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="I41">
         <f t="shared" ref="I41" si="2">I40*7/5</f>
-        <v>26.740000000000002</v>
+        <v>28.419999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1421,13 +1421,13 @@
       </c>
       <c r="I42">
         <f t="shared" ref="I42" si="3">I41/30</f>
-        <v>0.89133333333333342</v>
+        <v>0.94733333333333325</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J43" s="2">
         <f>K39/J39</f>
-        <v>0.61217948717948723</v>
+        <v>0.65064102564102566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminated some compiler warning messages.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -547,8 +547,8 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +744,9 @@
       <c r="H10">
         <v>8</v>
       </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1374,7 +1377,7 @@
       </c>
       <c r="I39">
         <f t="shared" ref="I39:K39" si="0">SUM(I2:I37)</f>
-        <v>101.5</v>
+        <v>103.5</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -1395,7 +1398,7 @@
       </c>
       <c r="I40">
         <f t="shared" ref="I40" si="1">I39/5</f>
-        <v>20.3</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1408,7 +1411,7 @@
       </c>
       <c r="I41">
         <f t="shared" ref="I41" si="2">I40*7/5</f>
-        <v>28.419999999999998</v>
+        <v>28.98</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1421,7 +1424,7 @@
       </c>
       <c r="I42">
         <f t="shared" ref="I42" si="3">I41/30</f>
-        <v>0.94733333333333325</v>
+        <v>0.96599999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on groundwater transport (GWT) in GHB package.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Package or feature</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>TS Actual</t>
+  </si>
+  <si>
+    <t>GWT Actual</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -544,11 +547,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +563,7 @@
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +597,11 @@
       <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -609,7 +615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -629,7 +635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -652,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -669,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -683,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -700,7 +706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -714,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -731,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -748,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -765,7 +771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -782,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -805,7 +811,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -828,7 +834,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -851,7 +857,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -874,7 +880,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -897,7 +903,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -920,7 +926,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -934,7 +940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -948,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -971,7 +977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -985,7 +991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1053,8 +1059,11 @@
       <c r="K25">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1092,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1170,7 +1179,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Worked on SSM for GWT.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +751,10 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
@@ -1386,7 +1389,7 @@
       </c>
       <c r="I39">
         <f t="shared" ref="I39:K39" si="0">SUM(I2:I37)</f>
-        <v>103.5</v>
+        <v>109.5</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -1407,7 +1410,7 @@
       </c>
       <c r="I40">
         <f t="shared" ref="I40" si="1">I39/5</f>
-        <v>20.7</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1420,7 +1423,7 @@
       </c>
       <c r="I41">
         <f t="shared" ref="I41" si="2">I40*7/5</f>
-        <v>28.98</v>
+        <v>30.659999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1433,7 +1436,7 @@
       </c>
       <c r="I42">
         <f t="shared" ref="I42" si="3">I41/30</f>
-        <v>0.96599999999999997</v>
+        <v>1.0219999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked on GWB export with MODFLOW 6 groundwater transport.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="L10">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
         <v>0.75</v>
       </c>
       <c r="L25">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on display of GHB GWT concentrations.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="L10">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
         <v>0.75</v>
       </c>
       <c r="L25">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
worked on GWT for Well package.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,6 +1239,9 @@
       <c r="K31">
         <v>0.75</v>
       </c>
+      <c r="L31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
Worked on Well package with GWT in MF6 Updated URLs for modeling programs.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0.75</v>
       </c>
       <c r="L31">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on GWT with RIV package in MF6
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,6 +1094,9 @@
       <c r="K26">
         <v>0.75</v>
       </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
Worked on GWT in CHD and RCH packages.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
+      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,6 +1213,9 @@
       <c r="K30">
         <v>1</v>
       </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1272,7 +1275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1300,8 +1303,11 @@
       <c r="K33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>101.5</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1419,7 +1425,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1432,7 +1438,7 @@
         <v>30.659999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>1.0219999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J43" s="2">
         <f>K39/J39</f>
         <v>0.65064102564102566</v>

</xml_diff>

<commit_message>
worked on GWT with EVT in MF6. Fixed minor bug in Import Gridded Data dialog box.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,6 +1335,9 @@
       <c r="K34">
         <v>1</v>
       </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">

</xml_diff>

<commit_message>
worked on supporting GWT in ETS package in MODFLOW 6.
</commit_message>
<xml_diff>
--- a/ModelMuse/MODFLOW 6 GWT planning.xlsx
+++ b/ModelMuse/MODFLOW 6 GWT planning.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>